<commit_message>
Updated cleaner anonymised data
</commit_message>
<xml_diff>
--- a/Copy of Sorted Questionnaire Results - sorted.xlsx
+++ b/Copy of Sorted Questionnaire Results - sorted.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/cs18416_bristol_ac_uk/Documents/Documents/Artemis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="313" documentId="8_{C722BE30-6AEC-4148-A7A1-CD6A100325AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADC57755-0918-477C-9F27-381E56D84811}"/>
+  <xr:revisionPtr revIDLastSave="314" documentId="8_{C722BE30-6AEC-4148-A7A1-CD6A100325AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9510F863-794C-4166-A311-7196144FCC8A}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6DEF699-F8DA-4270-8E18-411986556592}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$1:$D$157</definedName>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9548" uniqueCount="1663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9237" uniqueCount="1663">
   <si>
     <t>duration (in seconds)</t>
   </si>
@@ -5600,7 +5599,7 @@
   <dimension ref="A1:CU160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -53391,1896 +53390,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02607C7-FD1E-4E33-8468-E81ADCE79495}">
-  <dimension ref="A1:F157"/>
-  <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="I147" sqref="I147"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="90">
-      <c r="A1" s="1" t="s">
-        <v>1524</v>
-      </c>
-      <c r="F1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2">
-        <f>IF(OR(F2="", F2="i'd prefer not to say"),0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E66" si="0">IF(OR(F3="", F3="i'd prefer not to say"),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F29" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F31" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F33" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" t="s">
-        <v>60</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F34" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" t="s">
-        <v>60</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F35" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" t="s">
-        <v>60</v>
-      </c>
-      <c r="E36">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F36" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
-        <v>60</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F37" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" t="s">
-        <v>60</v>
-      </c>
-      <c r="E38">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F38" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" t="s">
-        <v>60</v>
-      </c>
-      <c r="E39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F39" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
-        <v>60</v>
-      </c>
-      <c r="E40">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>60</v>
-      </c>
-      <c r="E41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F41" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" t="s">
-        <v>60</v>
-      </c>
-      <c r="E42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F42" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" t="s">
-        <v>60</v>
-      </c>
-      <c r="E43">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F43" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>60</v>
-      </c>
-      <c r="E44">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F44" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" t="s">
-        <v>60</v>
-      </c>
-      <c r="E45">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F45" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" t="s">
-        <v>60</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F46" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" t="s">
-        <v>60</v>
-      </c>
-      <c r="E47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F47" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" t="s">
-        <v>60</v>
-      </c>
-      <c r="E48">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F48" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" t="s">
-        <v>60</v>
-      </c>
-      <c r="E49">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F49" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" t="s">
-        <v>60</v>
-      </c>
-      <c r="E50">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F50" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" t="s">
-        <v>60</v>
-      </c>
-      <c r="E51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F51" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" t="s">
-        <v>60</v>
-      </c>
-      <c r="E52">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F52" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" t="s">
-        <v>60</v>
-      </c>
-      <c r="E53">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F53" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" t="s">
-        <v>60</v>
-      </c>
-      <c r="E54">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F54" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" t="s">
-        <v>60</v>
-      </c>
-      <c r="E55">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F55" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" t="s">
-        <v>60</v>
-      </c>
-      <c r="E56">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F56" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" t="s">
-        <v>60</v>
-      </c>
-      <c r="E57">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F57" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" t="s">
-        <v>60</v>
-      </c>
-      <c r="E58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F58" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" t="s">
-        <v>60</v>
-      </c>
-      <c r="E59">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F59" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" t="s">
-        <v>60</v>
-      </c>
-      <c r="E60">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F60" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" t="s">
-        <v>60</v>
-      </c>
-      <c r="E61">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F61" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" t="s">
-        <v>60</v>
-      </c>
-      <c r="E62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F62" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" t="s">
-        <v>60</v>
-      </c>
-      <c r="E63">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F63" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" t="s">
-        <v>60</v>
-      </c>
-      <c r="E64">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F64" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" t="s">
-        <v>60</v>
-      </c>
-      <c r="E65">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F65" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" t="s">
-        <v>60</v>
-      </c>
-      <c r="E66">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F66" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" t="s">
-        <v>91</v>
-      </c>
-      <c r="E67">
-        <f t="shared" ref="E67:E130" si="1">IF(OR(F67="", F67="i'd prefer not to say"),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="F67" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" t="s">
-        <v>91</v>
-      </c>
-      <c r="E68">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F68" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" t="s">
-        <v>91</v>
-      </c>
-      <c r="E69">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F69" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" t="s">
-        <v>91</v>
-      </c>
-      <c r="E70">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F70" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" t="s">
-        <v>91</v>
-      </c>
-      <c r="E71">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F71" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" t="s">
-        <v>91</v>
-      </c>
-      <c r="E72">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F72" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" t="s">
-        <v>91</v>
-      </c>
-      <c r="E73">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F73" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" t="s">
-        <v>91</v>
-      </c>
-      <c r="E74">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F74" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75" t="s">
-        <v>91</v>
-      </c>
-      <c r="E75">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F75" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" t="s">
-        <v>91</v>
-      </c>
-      <c r="E76">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F76" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" t="s">
-        <v>91</v>
-      </c>
-      <c r="E77">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F77" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" t="s">
-        <v>91</v>
-      </c>
-      <c r="E78">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F78" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" t="s">
-        <v>91</v>
-      </c>
-      <c r="E79">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F79" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80" t="s">
-        <v>91</v>
-      </c>
-      <c r="E80">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F80" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
-      <c r="A81" t="s">
-        <v>91</v>
-      </c>
-      <c r="E81">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F81" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82" t="s">
-        <v>91</v>
-      </c>
-      <c r="E82">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F82" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="A83" t="s">
-        <v>91</v>
-      </c>
-      <c r="E83">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F83" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
-      <c r="A84" t="s">
-        <v>91</v>
-      </c>
-      <c r="E84">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F84" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
-      <c r="A85" t="s">
-        <v>91</v>
-      </c>
-      <c r="E85">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F85" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
-      <c r="A86" t="s">
-        <v>91</v>
-      </c>
-      <c r="E86">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F86" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="A87" t="s">
-        <v>91</v>
-      </c>
-      <c r="E87">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F87" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="A88" t="s">
-        <v>91</v>
-      </c>
-      <c r="E88">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F88" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89" t="s">
-        <v>91</v>
-      </c>
-      <c r="E89">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F89" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
-      <c r="A90" t="s">
-        <v>91</v>
-      </c>
-      <c r="E90">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F90" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
-      <c r="A91" t="s">
-        <v>91</v>
-      </c>
-      <c r="E91">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F91" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
-      <c r="A92" t="s">
-        <v>91</v>
-      </c>
-      <c r="E92">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F92" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
-      <c r="A93" t="s">
-        <v>91</v>
-      </c>
-      <c r="E93">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F93" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
-      <c r="A94" t="s">
-        <v>91</v>
-      </c>
-      <c r="E94">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F94" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95" t="s">
-        <v>91</v>
-      </c>
-      <c r="E95">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F95" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
-      <c r="A96" t="s">
-        <v>91</v>
-      </c>
-      <c r="E96">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F96" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
-      <c r="A97" t="s">
-        <v>91</v>
-      </c>
-      <c r="E97">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F97" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
-      <c r="A98" t="s">
-        <v>91</v>
-      </c>
-      <c r="E98">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F98" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
-      <c r="A99" t="s">
-        <v>91</v>
-      </c>
-      <c r="E99">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F99" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100" t="s">
-        <v>91</v>
-      </c>
-      <c r="E100">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F100" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
-      <c r="A101" t="s">
-        <v>91</v>
-      </c>
-      <c r="E101">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F101" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
-      <c r="A102" t="s">
-        <v>91</v>
-      </c>
-      <c r="E102">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F102" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6">
-      <c r="A103" t="s">
-        <v>91</v>
-      </c>
-      <c r="E103">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F103" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
-      <c r="A104" t="s">
-        <v>91</v>
-      </c>
-      <c r="E104">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F104" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
-      <c r="A105" t="s">
-        <v>91</v>
-      </c>
-      <c r="E105">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F105" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
-      <c r="A106" t="s">
-        <v>141</v>
-      </c>
-      <c r="E106">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F106" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
-      <c r="A107" t="s">
-        <v>141</v>
-      </c>
-      <c r="E107">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F107" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6">
-      <c r="A108" t="s">
-        <v>115</v>
-      </c>
-      <c r="E108">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F108" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6">
-      <c r="A109" t="s">
-        <v>115</v>
-      </c>
-      <c r="E109">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F109" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6">
-      <c r="A110" t="s">
-        <v>115</v>
-      </c>
-      <c r="E110">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F110" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
-      <c r="A111" t="s">
-        <v>115</v>
-      </c>
-      <c r="E111">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F111" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6">
-      <c r="A112" t="s">
-        <v>115</v>
-      </c>
-      <c r="E112">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F112" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6">
-      <c r="A113" t="s">
-        <v>115</v>
-      </c>
-      <c r="E113">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F113" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6">
-      <c r="A114" t="s">
-        <v>115</v>
-      </c>
-      <c r="E114">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F114" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
-      <c r="A115" t="s">
-        <v>115</v>
-      </c>
-      <c r="E115">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F115" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6">
-      <c r="A116" t="s">
-        <v>115</v>
-      </c>
-      <c r="E116">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F116" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
-      <c r="A117" t="s">
-        <v>115</v>
-      </c>
-      <c r="E117">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F117" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
-      <c r="A118" t="s">
-        <v>115</v>
-      </c>
-      <c r="E118">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F118" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
-      <c r="A119" t="s">
-        <v>115</v>
-      </c>
-      <c r="E119">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F119" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
-      <c r="A120" t="s">
-        <v>115</v>
-      </c>
-      <c r="E120">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F120" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6">
-      <c r="A121" t="s">
-        <v>115</v>
-      </c>
-      <c r="E121">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F121" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
-      <c r="A122" t="s">
-        <v>115</v>
-      </c>
-      <c r="E122">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F122" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
-      <c r="A123" t="s">
-        <v>115</v>
-      </c>
-      <c r="E123">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F123" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124" t="s">
-        <v>115</v>
-      </c>
-      <c r="E124">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F124" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6">
-      <c r="A125" t="s">
-        <v>115</v>
-      </c>
-      <c r="E125">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F125" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6">
-      <c r="A126" t="s">
-        <v>115</v>
-      </c>
-      <c r="E126">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F126" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6">
-      <c r="A127" t="s">
-        <v>115</v>
-      </c>
-      <c r="E127">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F127" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6">
-      <c r="A128" t="s">
-        <v>115</v>
-      </c>
-      <c r="E128">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F128" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6">
-      <c r="A129" t="s">
-        <v>115</v>
-      </c>
-      <c r="E129">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F129" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6">
-      <c r="A130" t="s">
-        <v>115</v>
-      </c>
-      <c r="E130">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F130" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6">
-      <c r="A131" t="s">
-        <v>115</v>
-      </c>
-      <c r="E131">
-        <f t="shared" ref="E131:E155" si="2">IF(OR(F131="", F131="i'd prefer not to say"),0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="F131" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6">
-      <c r="A132" t="s">
-        <v>115</v>
-      </c>
-      <c r="E132">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F132" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6">
-      <c r="A133" t="s">
-        <v>115</v>
-      </c>
-      <c r="E133">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F133" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6">
-      <c r="A134" t="s">
-        <v>115</v>
-      </c>
-      <c r="E134">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F134" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6">
-      <c r="A135" t="s">
-        <v>115</v>
-      </c>
-      <c r="E135">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F135" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6">
-      <c r="A136" t="s">
-        <v>115</v>
-      </c>
-      <c r="E136">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F136" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6">
-      <c r="A137" t="s">
-        <v>115</v>
-      </c>
-      <c r="E137">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F137" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6">
-      <c r="A138" t="s">
-        <v>115</v>
-      </c>
-      <c r="E138">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F138" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6">
-      <c r="A139" t="s">
-        <v>115</v>
-      </c>
-      <c r="E139">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F139" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6">
-      <c r="A140" t="s">
-        <v>115</v>
-      </c>
-      <c r="E140">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F140" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6">
-      <c r="A141" t="s">
-        <v>115</v>
-      </c>
-      <c r="E141">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F141" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6">
-      <c r="A142" t="s">
-        <v>115</v>
-      </c>
-      <c r="E142">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F142" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6">
-      <c r="A143" t="s">
-        <v>115</v>
-      </c>
-      <c r="E143">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F143" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6">
-      <c r="A144" t="s">
-        <v>115</v>
-      </c>
-      <c r="E144">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F144" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6">
-      <c r="A145" t="s">
-        <v>115</v>
-      </c>
-      <c r="E145">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F145" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6">
-      <c r="A146" t="s">
-        <v>115</v>
-      </c>
-      <c r="E146">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F146" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6">
-      <c r="A147" t="s">
-        <v>115</v>
-      </c>
-      <c r="E147">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F147" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6">
-      <c r="A148" t="s">
-        <v>115</v>
-      </c>
-      <c r="E148">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F148" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6">
-      <c r="A149" t="s">
-        <v>115</v>
-      </c>
-      <c r="E149">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F149" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6">
-      <c r="A150" t="s">
-        <v>115</v>
-      </c>
-      <c r="E150">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F150" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6">
-      <c r="A151" t="s">
-        <v>115</v>
-      </c>
-      <c r="E151">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F151" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6">
-      <c r="A152" t="s">
-        <v>115</v>
-      </c>
-      <c r="E152">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F152" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6">
-      <c r="A153" t="s">
-        <v>115</v>
-      </c>
-      <c r="E153">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F153" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6">
-      <c r="A154" t="s">
-        <v>115</v>
-      </c>
-      <c r="E154">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F154" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6">
-      <c r="A155" t="s">
-        <v>115</v>
-      </c>
-      <c r="E155">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F155" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6">
-      <c r="A156" t="s">
-        <v>115</v>
-      </c>
-      <c r="E156">
-        <f>SUM(E2:E155)</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6">
-      <c r="A157" t="e">
-        <f>AVERAGE(A2:A79)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A157">
-    <sortCondition ref="A1:A157"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>